<commit_message>
Updated the linkage so should match main, and added a few datasets that were over looked
</commit_message>
<xml_diff>
--- a/BHF_Dashboards/BHF_DSC_TRE_External_Dashboard/Archive/Lars_module/Wales_scraping.xlsx
+++ b/BHF_Dashboards/BHF_DSC_TRE_External_Dashboard/Archive/Lars_module/Wales_scraping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LarsMurdock\Documents\Repo\BHF_DSC_HDS\BHF_Dashboards\BHF_DSC_TRE_External_Dashboard\Archive\Lars_module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15918DA-AAE5-4E3A-B083-F097ECAFC65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA62725-56E4-4223-B6B0-D6AE0D06CEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="7" xr2:uid="{280FE3C0-9181-4AA4-8326-DD57F94C9FFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="10" xr2:uid="{280FE3C0-9181-4AA4-8326-DD57F94C9FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="CCDS" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="DF_SHIELDED_PATIENTS" sheetId="8" r:id="rId6"/>
     <sheet name="DEATHS" sheetId="9" r:id="rId7"/>
     <sheet name="ICNARC_LINKAGE" sheetId="10" r:id="rId8"/>
-    <sheet name="CARE_HOMES_20200708" sheetId="11" r:id="rId9"/>
+    <sheet name="Outpatient Referral (OPRD)" sheetId="12" r:id="rId9"/>
+    <sheet name="CARE_HOMES_20200708" sheetId="11" r:id="rId10"/>
+    <sheet name="cog_2020-04-24_metadata" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1285">
   <si>
     <t>Description to follow</t>
   </si>
@@ -3560,6 +3562,345 @@
   </si>
   <si>
     <t>Encrypted unique record number (URN) of the care home. Note that the unencrypted URN links to a specific care home from the care inspectorate Wales list.</t>
+  </si>
+  <si>
+    <t>Lower Layer Super Output Area (LSOA) code (9 characters) in which the patient is resident, based on the previous census.</t>
+  </si>
+  <si>
+    <t>SOURCE_OF_REF_DESC</t>
+  </si>
+  <si>
+    <t>Source of Referral Description. This is a classification which is used to identify the source of referral of each Outpatient Episode or Outpatient Referral.</t>
+  </si>
+  <si>
+    <t>Previous Organisation Code (3 character code). Code for the Local Health Board (LHB) where the patient is resident, identified via the NHS Postcode Directory.This ensures that the Local Health Board can receive information about the care given to its residents. Based on the previous census. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>PAT_REG_ORG_COUNTRYNAME</t>
+  </si>
+  <si>
+    <t>CLIN_REF_DT</t>
+  </si>
+  <si>
+    <t>The Clinical Referral Date (CRD) is the clinically significant date marking the start of a period of waiting either for an initial outpatient consultation or for an episode of treatment such as elective surgery. The CRD is used to order pick lists used for booking patients, and it does not change under any circumstances. It is not used to calculate performance waiting times statistics. Note: For outpatient data, the Clinical Referral Date (CRD) is the date that the referral of an outpatient appointment is received in the Local Health Board/Trust. All referrals should be date stamped on opening – this date stamp is the CRD. In addition, this CRD must be entered into PAS on the same day. If the referral request takes the form of a phone call followed by a letter, record the date when the letter arrives. If there is no following letter, the date of the verbal request should be recorded. Note: For inpatient and day cases, the Clinical Referral Date (CRD) is the date that a decision was made by the clinician within the Local Health Board/Trust (or GP outside the Local Health Board/Trust in cases of direct access referrals) to list the patient for treatment. The CRD is used to order the waiting list selection of patients.</t>
+  </si>
+  <si>
+    <t>Referring Organisation Name. The name of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral. This information is essential for managing contracts which are based on patterns of referral.</t>
+  </si>
+  <si>
+    <t>Encrypted Local Patient Identifier. This is the case record number. It is a unique identifier for a patient within a health care provider. Where care for NHS patients is sub-commissioned in the independent sector or overseas, the NHS commissioner local patient identifier should be used. If no NHS local patient identifier has been assigned the independent sector or overseas provider identifier should be used.</t>
+  </si>
+  <si>
+    <t>REF_DT_KEY</t>
+  </si>
+  <si>
+    <t>SOURCE_OF_REF_DERIVED_CD</t>
+  </si>
+  <si>
+    <t>Derived Source of Referral Code. This is a classification which is used to identify the source of referral of each Outpatient Episode or Outpatient Referral.</t>
+  </si>
+  <si>
+    <t>SOURCE_OF_REF_DERIVED_DESC</t>
+  </si>
+  <si>
+    <t>Derived Source of Referral Description. This is a classification which is used to identify the source of referral of each Outpatient Episode or Outpatient Referral.</t>
+  </si>
+  <si>
+    <t>Current Country Name of the refering organisation.</t>
+  </si>
+  <si>
+    <t>PAT_REF_AGE_TEN_YEAR_BANDS</t>
+  </si>
+  <si>
+    <t>The ten year age band of the patient at date of patient referral.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_GEO_HEALTH_ORG_NAME</t>
+  </si>
+  <si>
+    <t>Local Authority code (9 characters) in which the patient is resident. Based on the current census.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_ORG_CD</t>
+  </si>
+  <si>
+    <t>This is the code (6 characters) of the patient's registered General Practitioner (GP) Practice. This allows the practice to be notified about treatment received by the patient. The registered GP Practice may or may not be the same as the referring GP Practice.</t>
+  </si>
+  <si>
+    <t>Treatment Function Categroy. The category of the treatment function code.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_GEO_HEALTH_ORG_PREVIOUS_CD</t>
+  </si>
+  <si>
+    <t>PAT_REF_AGE_YEARS</t>
+  </si>
+  <si>
+    <t>The age in years of patient at date of patient referral.</t>
+  </si>
+  <si>
+    <t>Derived code indication the sex of the person, employee or patient.</t>
+  </si>
+  <si>
+    <t>Derived Organisation Name. Name of the Local Health Board (LHB) where the patient is a resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>SOURCE_OF_REF_CD</t>
+  </si>
+  <si>
+    <t>Source of Referral Code. This is a classification which is used to identify the source of referral of each Outpatient Episode or Outpatient Referral.</t>
+  </si>
+  <si>
+    <t>REF_ORG_CURR_CD_WELSH_ONLY</t>
+  </si>
+  <si>
+    <t>Current Referring Site Code (5 character code), for referring organisations in Wales only. The code of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral. This information is essential for managing contracts which are based on patterns of referral.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_UA_NAME</t>
+  </si>
+  <si>
+    <t>REF_STAFF_PSEUDO</t>
+  </si>
+  <si>
+    <t>Pseudonymised Referrer Staff Code. This is the nationally recognized code of the person making the referral. This may be a General Medical Practitioner (GMP), General Dental Practitioner (GDP), Consultant or Independent Nurse.</t>
+  </si>
+  <si>
+    <t>SERVICE_TYPE_REQST_DERIVED_CD</t>
+  </si>
+  <si>
+    <t>Derived Service Type Requested Code. The terms of reference for the referral request.</t>
+  </si>
+  <si>
+    <t>Organisation Code (9 characters). Code for the Local Health Board (LHB) where the patient is a resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Based on the current census. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>Country code (9 character) in which the patient is resident, based on the current census.</t>
+  </si>
+  <si>
+    <t>Current Referring Organisation Name. The name of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral. This information is essential for managing contracts which are based on patterns of referral.</t>
+  </si>
+  <si>
+    <t>CON_SPEC_DERIVED_CD</t>
+  </si>
+  <si>
+    <t>Derived Consultant Main Speciality Code. A unique code identifying each Main Specialty designated by Royal Colleges. Specialties are divisions of clinical work which may be defined by body systems (dermatology), age (paediatrics), clinical technology (nuclear medicine), clinical function (rheumatology), group of diseases (oncology) or combinations of these factors.Only Specialty titles recognised by the Royal Colleges and Faculties should be used. This list is maintained by the General and Specialist Medical Practice (Education, Training and Qualifications) Order 2003 and European Primary and Specialist Dental Qualifications Regulations 1998. Each consultant should be assigned a Main Specialty by the organisation to which the consultant is contracted. For physicians and surgeons with a generalist component to their work, the Main Specialty should be general medicine or general surgery. The hallmark of a general physician or general surgeon is the continued care of unselected emergency referrals. The Main Specialty is specific to a Health Care Provider. If, for example, a consultant physician working in two Health Care Providers has a generalist component to the work in one and not the other, general medicine is only assigned as the Main Specialty in the former case. Consultants in general medicine or general surgery may also have specialist interests and these should be recorded as well as the Main Specialty. The initial source of the information should be the designation on the consultant's contract. This should be checked periodically against the work a consultant is actually doing so that the statistics can relate to a consultant's current type of work. The Main Specialty only should be used for the purpose of producing Specialty costing statistics and for Workforce statistics where links with activity and finance are required. Other specialist interests of consultants may be recorded for workforce planning purposes. The Main Specialty code for general practitioners is General Medical Practice or General Dental Practice. Joint Consultant Clinic activity should be recorded against the Main Specialty code of the consultant managing the clinic.</t>
+  </si>
+  <si>
+    <t>CON_SPEC_CAT</t>
+  </si>
+  <si>
+    <t>Consultant Speciality Category. The category of the consultant's main speciality.</t>
+  </si>
+  <si>
+    <t>PAT_CLIN_REF_AGE_TEN_YEAR_BANDS</t>
+  </si>
+  <si>
+    <t>The ten year age band of the patient at date of clinical referral.</t>
+  </si>
+  <si>
+    <t>Referring Site Code (5 character code). The code of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral. This information is essential for managing contracts which are based on patterns of referral.</t>
+  </si>
+  <si>
+    <t>Description of the sex of the person, employee or patient.</t>
+  </si>
+  <si>
+    <t>Previous Organisation Code (3 character code). Code for the Local Health Board (LHB) where the patient is resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>COUNT_EFF_GP_REF_RATE_NUMERATOR</t>
+  </si>
+  <si>
+    <t>Current Organisation Name. Name of the Local Health Board (LHB) where the patient is a resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>PAT_REF_AGE_FIVE_YEAR_BANDS</t>
+  </si>
+  <si>
+    <t>The five year age band of the patient at date of patient referral.</t>
+  </si>
+  <si>
+    <t>DUR_REF_CLIN_REF_DAYS</t>
+  </si>
+  <si>
+    <t>The total number of days between the patient referral date and the clinical referral date.</t>
+  </si>
+  <si>
+    <t>PAT_CLIN_REF_AGE_YEARS</t>
+  </si>
+  <si>
+    <t>The age in years of patient at date of clinical referral.</t>
+  </si>
+  <si>
+    <t>PAT_STATS_CURR_CENSUS_HEALTH_ORG_PREV_CD</t>
+  </si>
+  <si>
+    <t>Previous Organisation Code (3 characters). Code for the Local Health Board (LHB) where the patient is a resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Based on the current census. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>Local Authority code (9 characters) in which the patient is resident. Based on the previous census.</t>
+  </si>
+  <si>
+    <t>Organisation Code (9 characters). Code for the Local Health Board (LHB) where the patient is a resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Based on the previous census. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>SERVICE_TYPE_REQST_DESC</t>
+  </si>
+  <si>
+    <t>Service Type Requested Description. The terms of reference for the referral request.</t>
+  </si>
+  <si>
+    <t>Lower Layer Super Output Area (LSOA) code (9 characters) in which the patient is resident, for the latest version of LSOA codes (2011)</t>
+  </si>
+  <si>
+    <t>CON_SPEC_CD</t>
+  </si>
+  <si>
+    <t>Consultant Main Speciality Code. A unique code identifying each Main Specialty designated by Royal Colleges. Specialties are divisions of clinical work which may be defined by body systems (dermatology), age (paediatrics), clinical technology (nuclear medicine), clinical function (rheumatology), group of diseases (oncology) or combinations of these factors.Only Specialty titles recognised by the Royal Colleges and Faculties should be used. This list is maintained by the General and Specialist Medical Practice (Education, Training and Qualifications) Order 2003 and European Primary and Specialist Dental Qualifications Regulations 1998. Each consultant should be assigned a Main Specialty by the organisation to which the consultant is contracted. For physicians and surgeons with a generalist component to their work, the Main Specialty should be general medicine or general surgery. The hallmark of a general physician or general surgeon is the continued care of unselected emergency referrals. The Main Specialty is specific to a Health Care Provider. If, for example, a consultant physician working in two Health Care Providers has a generalist component to the work in one and not the other, general medicine is only assigned as the Main Specialty in the former case. Consultants in general medicine or general surgery may also have specialist interests and these should be recorded as well as the Main Specialty. The initial source of the information should be the designation on the consultant's contract. This should be checked periodically against the work a consultant is actually doing so that the statistics can relate to a consultant's current type of work. The Main Specialty only should be used for the purpose of producing Specialty costing statistics and for Workforce statistics where links with activity and finance are required. Other specialist interests of consultants may be recorded for workforce planning purposes. The Main Specialty code for general practitioners is General Medical Practice or General Dental Practice. Joint Consultant Clinic activity should be recorded against the Main Specialty code of the consultant managing the clinic.</t>
+  </si>
+  <si>
+    <t>COUNT_OUTPATIENT_REF</t>
+  </si>
+  <si>
+    <t>REF_ORG_CURR_NAME_WELSH_ONLY</t>
+  </si>
+  <si>
+    <t>Current Referring Organisation Name, for referring organisations in Wales only. The name of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral.</t>
+  </si>
+  <si>
+    <t>Previous Organisation Name. Name for the Local Health Board (LHB) where the patient is resident, identified via the NHS Postcode Directory. This ensures that the Local Health Board can receive information about the care given to its residents. Note: For English Residents treated in Wales, use the Organisation Code of the Primary Care Trust (PCT) of Residence for all activity / waiting times data up to 31st March 2013. From 1st April 2013 (inclusive) onwards, use the Organisation Code of the Clinical Commissioning Group (CCG).</t>
+  </si>
+  <si>
+    <t>PAT_CLIN_REF_AGE_FIVE_YEAR_BANDS</t>
+  </si>
+  <si>
+    <t>The five year age band of the patient at date of clinical referral.</t>
+  </si>
+  <si>
+    <t>CON_SPEC_DESC</t>
+  </si>
+  <si>
+    <t>Consultant Main Speciality Description. Descriptions for each Main Specialty designated by Royal Colleges. Specialties are divisions of clinical work which may be defined by body systems (dermatology), age (paediatrics), clinical technology (nuclear medicine), clinical function (rheumatology), group of diseases (oncology) or combinations of these factors.Only Specialty titles recognised by the Royal Colleges and Faculties should be used. This list is maintained by the General and Specialist Medical Practice (Education, Training and Qualifications) Order 2003 and European Primary and Specialist Dental Qualifications Regulations 1998. Each consultant should be assigned a Main Specialty by the organisation to which the consultant is contracted. For physicians and surgeons with a generalist component to their work, the Main Specialty should be general medicine or general surgery. The hallmark of a general physician or general surgeon is the continued care of unselected emergency referrals. The Main Specialty is specific to a Health Care Provider. If, for example, a consultant physician working in two Health Care Providers has a generalist component to the work in one and not the other, general medicine is only assigned as the Main Specialty in the former case. Consultants in general medicine or general surgery may also have specialist interests and these should be recorded as well as the Main Specialty. The initial source of the information should be the designation on the consultant's contract. This should be checked periodically against the work a consultant is actually doing so that the statistics can relate to a consultant's current type of work. The Main Specialty only should be used for the purpose of producing Specialty costing statistics and for Workforce statistics where links with activity and finance are required. Other specialist interests of consultants may be recorded for workforce planning purposes. The Main Specialty code for general practitioners is General Medical Practice or General Dental Practice. Joint Consultant Clinic activity should be recorded against the Main Specialty code of the consultant managing the clinic.</t>
+  </si>
+  <si>
+    <t>REF_DT_VALID</t>
+  </si>
+  <si>
+    <t>Indiactes whether or not the patient referral date is valid.</t>
+  </si>
+  <si>
+    <t>REASON_FOR_REF</t>
+  </si>
+  <si>
+    <t>The reason(s) for the patient requiring involvement with care professionals. These may include any problem, issue or event affecting the patient's health and/ or well being. The information held within this data item must be a valid clinical code or term.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_GEO_HEALTH_ORG_PREVIOUS_NAME</t>
+  </si>
+  <si>
+    <t>Current Referring Site Code (5 character code). The code of the organisation of the General Medical Practitioner (GMP), General Dental Practitioner (GDP) and Consultant or Independent Nurse making the referral. This information is essential for managing contracts which are based on patterns of referral.</t>
+  </si>
+  <si>
+    <t>REF_DT</t>
+  </si>
+  <si>
+    <t>This is the date on which the patient was told about the referral. The starting point should be the date of referral given on the referral notification (not the date the letter was received in hospital). In cases where the referrer fails to specify a date of referral, the date the referral notification was received should be used. Dates to be used; - Date the patient is told about the referral - Date on referral notification - Date of receipt of referral notification (only to be used where no date on document present) - Date of verbal referral – For verbal referrals, the date of referral is equal to the date on which the verbal request is received. This date must be documented; any follow up written referral documentation will not affect the verbal date of referral. - Where a patient self refers, the date of referral is equal to the date of attendance.</t>
+  </si>
+  <si>
+    <t>CLIN_REF_DT_VALID</t>
+  </si>
+  <si>
+    <t>Indiactes whether or not the clinical referral date is valid.</t>
+  </si>
+  <si>
+    <t>Previous Local Authority code (4 characters) in which the patient is resident. Based on the current census.</t>
+  </si>
+  <si>
+    <t>PAT_REG_GP_GEO_HEALTH_ORG_CD</t>
+  </si>
+  <si>
+    <t>REF_PRIORITY_TYPE_DESC</t>
+  </si>
+  <si>
+    <t>Referrer Priority Type Description. This is the Referrer's assessment of the priority of a request for services. The value may be obtained from the text in the referral notification and is unaffected by the priority as assessed by the Consultant or Independent Nurse responsible for the outpatient appointment on review of the referral notification. Note: If a patient self-refers, this field should be populated with the default value of 1. Note: The 'routine' value is to be utilized as a default if no urgency or clinical priority is included within the referral notification. Where an urgency or clinical priority is included 'urgency' can be defined as per the extant guidance.</t>
+  </si>
+  <si>
+    <t>Previous Local Authority code (4 characters) in which the patient is resident. Based on the previous census.</t>
+  </si>
+  <si>
+    <t>SERVICE_TYPE_REQST_CD</t>
+  </si>
+  <si>
+    <t>Service Type Requested Code. The terms of reference for the referral request.</t>
+  </si>
+  <si>
+    <t>CLIN_REF_DT_KEY</t>
+  </si>
+  <si>
+    <t>REF_PRIORITY_TYPE_DERIVED_CD</t>
+  </si>
+  <si>
+    <t>Derived Referrer Priority Type Code. This is the Referrer's assessment of the priority of a request for services. The value may be obtained from the text in the referral notification and is unaffected by the priority as assessed by the Consultant or Independent Nurse responsible for the outpatient appointment on review of the referral notification. Note: If a patient self-refers, this field should be populated with the default value of 1. Note: The 'routine' value is to be utilized as a default if no urgency or clinical priority is included within the referral notification. Where an urgency or clinical priority is included 'urgency' can be defined as per the extant guidance.</t>
+  </si>
+  <si>
+    <t>REF_PRIORITY_TYPE_CD</t>
+  </si>
+  <si>
+    <t>Referrer Priority Type Code. This is the Referrer's assessment of the priority of a request for services. The value may be obtained from the text in the referral notification and is unaffected by the priority as assessed by the Consultant or Independent Nurse responsible for the outpatient appointment on review of the referral notification. Note: If a patient self-refers, this field should be populated with the default value of 1. Note: The 'routine' value is to be utilized as a default if no urgency or clinical priority is included within the referral notification. Where an urgency or clinical priority is included 'urgency' can be defined as per the extant guidance.</t>
+  </si>
+  <si>
+    <t>Country code (9 character) in which the patient is resident, based on the previous census.</t>
+  </si>
+  <si>
+    <t>sequence_name</t>
+  </si>
+  <si>
+    <t>Name of the viral sequence</t>
+  </si>
+  <si>
+    <t>Data typeText</t>
+  </si>
+  <si>
+    <t>lineage_support</t>
+  </si>
+  <si>
+    <t>Lineage Support</t>
+  </si>
+  <si>
+    <t>sample_date</t>
+  </si>
+  <si>
+    <t>Sample Date</t>
+  </si>
+  <si>
+    <t>lineage</t>
+  </si>
+  <si>
+    <t>Viral lineage</t>
+  </si>
+  <si>
+    <t>Data typeCoding</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Country collected</t>
+  </si>
+  <si>
+    <t>adm1</t>
+  </si>
+  <si>
+    <t>Nation of first adission</t>
+  </si>
+  <si>
+    <t>epi_week</t>
+  </si>
+  <si>
+    <t>Episode Week</t>
+  </si>
+  <si>
+    <t>Data typeNumber</t>
   </si>
 </sst>
 </file>
@@ -6550,6 +6891,321 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BC231D-2754-4C34-95FC-11B28F0ACC47}">
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28483EA6-4C1A-4858-A247-73FE35B17D3C}">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAEFCE3-B698-4285-974A-FBF3CA4D2677}">
   <dimension ref="A1:A87"/>
@@ -10441,7 +11097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7C4BF5-7DBA-436F-81C1-9B6765457FBB}">
   <dimension ref="A1:A687"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -13888,68 +14544,68 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BC231D-2754-4C34-95FC-11B28F0ACC47}">
-  <dimension ref="A1:A36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AC0B1E-4ADF-4AC1-A6BB-17FCD4B346AF}">
+  <dimension ref="A1:A315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1152</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1153</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1154</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1155</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1156</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1157</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -13959,87 +14615,87 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1161</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1162</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1163</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1164</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1166</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1167</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1168</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -14049,32 +14705,1427 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>575</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1169</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1171</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>